<commit_message>
update overtime and nhan vien ca lam viec
</commit_message>
<xml_diff>
--- a/ASP.NET CORE/HRMNS/Note.xlsx
+++ b/ASP.NET CORE/HRMNS/Note.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Dang Ky ca lam viec" sheetId="1" r:id="rId1"/>
+    <sheet name="Đang ly OT" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -21,6 +22,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>- Status phải tự chuyển sang active khi trong thời gian ca lam việc.Hết thời gian làm việc chuyển qua Inactive</t>
+  </si>
+  <si>
+    <t>- Vơi user dưới xưởng thì khi import phải check thời gian ca lam việc xem đúng không.</t>
+  </si>
+  <si>
+    <t>- Sau m10 hàng tháng sẽ chuyển danh sách dang ký OT : passed -&gt;Y, chỉ hiển thị passed = 'N'</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -54,8 +69,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -71,6 +87,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>166494</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1" y="190500"/>
+          <a:ext cx="5486400" cy="2261994"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -336,14 +395,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A16:A17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>